<commit_message>
Performance & Air Quality Data
</commit_message>
<xml_diff>
--- a/DSA210_DATA.xlsx
+++ b/DSA210_DATA.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
   <si>
     <t>Date</t>
   </si>
@@ -886,7 +886,7 @@
   <dimension ref="A1:I47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1461,7 +1461,7 @@
         <v>14.3</v>
       </c>
       <c r="C20" s="2">
-        <v>92</v>
+        <v>107</v>
       </c>
       <c r="D20" s="2">
         <v>26.1</v>
@@ -1490,7 +1490,7 @@
         <v>13.8</v>
       </c>
       <c r="C21" s="2">
-        <v>87</v>
+        <v>156</v>
       </c>
       <c r="D21" s="2">
         <v>24.9</v>
@@ -1519,7 +1519,7 @@
         <v>14</v>
       </c>
       <c r="C22" s="2">
-        <v>83</v>
+        <v>165</v>
       </c>
       <c r="D22" s="2">
         <v>23.5</v>
@@ -1751,7 +1751,7 @@
         <v>11</v>
       </c>
       <c r="C30" s="2">
-        <v>86</v>
+        <v>104</v>
       </c>
       <c r="D30" s="2">
         <v>25.6</v>
@@ -1867,7 +1867,7 @@
         <v>14.5</v>
       </c>
       <c r="C34" s="2">
-        <v>88</v>
+        <v>159</v>
       </c>
       <c r="D34" s="2">
         <v>26.5</v>
@@ -1908,7 +1908,7 @@
         <v>69</v>
       </c>
       <c r="G35" s="2">
-        <v>4.8</v>
+        <v>3</v>
       </c>
       <c r="H35" s="2">
         <v>6.1</v>
@@ -2070,7 +2070,7 @@
         <v>12.1</v>
       </c>
       <c r="C41" s="2">
-        <v>76</v>
+        <v>103</v>
       </c>
       <c r="D41" s="2">
         <v>20.5</v>
@@ -2099,7 +2099,7 @@
         <v>11.3</v>
       </c>
       <c r="C42" s="2">
-        <v>82</v>
+        <v>100</v>
       </c>
       <c r="D42" s="2">
         <v>23.6</v>
@@ -2110,14 +2110,14 @@
       <c r="F42" s="2">
         <v>77</v>
       </c>
-      <c r="G42" s="2">
-        <v>5.4</v>
-      </c>
-      <c r="H42" s="2">
-        <v>6.28</v>
-      </c>
-      <c r="I42" s="2">
-        <v>152</v>
+      <c r="G42" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H42" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I42" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
@@ -2157,7 +2157,7 @@
         <v>132</v>
       </c>
       <c r="C44" s="2">
-        <v>105</v>
+        <v>129</v>
       </c>
       <c r="D44" s="2">
         <v>27.4</v>
@@ -2186,7 +2186,7 @@
         <v>9.6999999999999993</v>
       </c>
       <c r="C45" s="2">
-        <v>89</v>
+        <v>167</v>
       </c>
       <c r="D45" s="2">
         <v>26.8</v>
@@ -2211,7 +2211,9 @@
       <c r="A46" s="1">
         <v>45770</v>
       </c>
-      <c r="B46" s="2"/>
+      <c r="B46" s="2">
+        <v>11</v>
+      </c>
       <c r="C46" s="2">
         <v>79</v>
       </c>
@@ -2263,5 +2265,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>